<commit_message>
Update 3rd order WENO coefficients calculator
</commit_message>
<xml_diff>
--- a/doc/Result_Record.xlsx
+++ b/doc/Result_Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Models\FVM\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309EB467-FF6C-412C-865B-B39D5E869A20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1EA1F6-A481-49E8-A401-B075A458DF04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1116" windowWidth="16650" windowHeight="10206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5934" yWindow="828" windowWidth="16650" windowHeight="10206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5th" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
   <si>
     <t>L1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +61,10 @@
   </si>
   <si>
     <t>Poly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WENO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,15 +391,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="4" width="9.84765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="9.84765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.84765625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.44921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -686,7 +692,7 @@
         <v>-0.41858005509210544</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -703,7 +709,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -717,7 +723,7 @@
         <v>2.90312201992803E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -731,7 +737,7 @@
         <v>3.6769991844076998E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -745,7 +751,7 @@
         <v>1.41552499787276E-8</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -762,7 +768,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -773,7 +779,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -784,7 +790,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -795,7 +801,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -817,20 +823,20 @@
       <c r="H29" t="s">
         <v>6</v>
       </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
       <c r="J29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L29">
-        <v>0.5</v>
-      </c>
-      <c r="M29">
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -852,24 +858,24 @@
       <c r="H30" t="s">
         <v>0</v>
       </c>
-      <c r="J30" s="1">
+      <c r="I30" s="1">
         <f>LOG(B30/C30)/LOG(B29/C29)</f>
         <v>5.0019572986932817</v>
       </c>
+      <c r="J30" s="1">
+        <f>LOG(C30/D30)/LOG(2)</f>
+        <v>5.0001899251177537</v>
+      </c>
       <c r="K30" s="1">
-        <f t="shared" ref="K30:M32" si="8">LOG(C30/D30)/LOG(2)</f>
-        <v>5.0001899251177537</v>
+        <f>LOG(D30/E30)/LOG(2)</f>
+        <v>4.9968995905353069</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="8"/>
-        <v>4.9968995905353069</v>
-      </c>
-      <c r="M30" s="1">
-        <f t="shared" si="8"/>
+        <f>LOG(E30/F30)/LOG(2)</f>
         <v>4.8695819266585314</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -891,24 +897,24 @@
       <c r="H31" t="s">
         <v>1</v>
       </c>
-      <c r="J31" s="1">
+      <c r="I31" s="1">
         <f>LOG(B31/C31)/LOG(B29/C29)</f>
         <v>4.9873252231915997</v>
       </c>
+      <c r="J31" s="1">
+        <f>LOG(C31/D31)/LOG(2)</f>
+        <v>4.9873343202422795</v>
+      </c>
       <c r="K31" s="1">
-        <f t="shared" si="8"/>
-        <v>4.9873343202422795</v>
+        <f>LOG(D31/E31)/LOG(2)</f>
+        <v>4.9966193879584422</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="8"/>
-        <v>4.9966193879584422</v>
-      </c>
-      <c r="M31" s="1">
-        <f t="shared" si="8"/>
+        <f>LOG(E31/F31)/LOG(2)</f>
         <v>4.9696532233440047</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -930,21 +936,208 @@
       <c r="H32" t="s">
         <v>2</v>
       </c>
-      <c r="J32" s="1">
+      <c r="I32" s="1">
         <f>LOG(B32/C32)/LOG(B29/C29)</f>
         <v>5.0011284146879769</v>
       </c>
+      <c r="J32" s="1">
+        <f>LOG(C32/D32)/LOG(2)</f>
+        <v>5.007444255036746</v>
+      </c>
       <c r="K32" s="1">
+        <f>LOG(D32/E32)/LOG(2)</f>
+        <v>5.003557125691878</v>
+      </c>
+      <c r="L32" s="1">
+        <f>LOG(E32/F32)/LOG(2)</f>
+        <v>5.0468770249812334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>4.5</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0.5</v>
+      </c>
+      <c r="F35">
+        <v>0.25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>0.5</v>
+      </c>
+      <c r="L35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>7.8192776413125699E-6</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1.08124282793362E-7</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3.6421202685985199E-9</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1.60302015969463E-10</v>
+      </c>
+      <c r="F36" s="1">
+        <v>8.5089984231142698E-12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <f>LOG(B36/C36)/LOG(B35/C35)</f>
+        <v>5.2792041020603531</v>
+      </c>
+      <c r="J36" s="1">
+        <f>LOG(C36/D36)/LOG(2)</f>
+        <v>4.8917681897318355</v>
+      </c>
+      <c r="K36" s="1">
+        <f>LOG(D36/E36)/LOG(2)</f>
+        <v>4.5059140890301954</v>
+      </c>
+      <c r="L36" s="1">
+        <f>LOG(E36/F36)/LOG(2)</f>
+        <v>4.2356594336079514</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.0676656261578601E-5</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1.45635883906296E-7</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4.6658453459182704E-9</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.90415033037408E-10</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1.00399432349302E-11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <f>LOG(B37/C37)/LOG(B35/C35)</f>
+        <v>5.2960234218572477</v>
+      </c>
+      <c r="J37" s="1">
+        <f>LOG(C37/D37)/LOG(2)</f>
+        <v>4.9640835729341539</v>
+      </c>
+      <c r="K37" s="1">
+        <f>LOG(D37/E37)/LOG(2)</f>
+        <v>4.6149192012636178</v>
+      </c>
+      <c r="L37" s="1">
+        <f>LOG(E37/F37)/LOG(2)</f>
+        <v>4.2453243646400596</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2.1363851494202999E-5</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.7809675945248101E-7</v>
+      </c>
+      <c r="D38" s="1">
+        <v>8.09095568460738E-9</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3.6509663150453699E-10</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1.8631351385503401E-11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1">
+        <f>LOG(B38/C38)/LOG(B35/C35)</f>
+        <v>5.3537115705929885</v>
+      </c>
+      <c r="J38" s="1">
+        <f>LOG(C38/D38)/LOG(2)</f>
+        <v>5.1031330029669109</v>
+      </c>
+      <c r="K38" s="1">
+        <f>LOG(D38/E38)/LOG(2)</f>
+        <v>4.4699598572643993</v>
+      </c>
+      <c r="L38" s="1">
+        <f>LOG(E38/F38)/LOG(2)</f>
+        <v>4.2924741320713302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="C40" s="1">
+        <f>(C36-C30)/C30*100</f>
+        <v>-52.268651581936389</v>
+      </c>
+      <c r="D40" s="1">
+        <f>(D36-D30)/D30*100</f>
+        <v>-48.543303887664656</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="C41" s="1">
+        <f t="shared" ref="C41:D41" si="8">(C37-C31)/C31*100</f>
+        <v>-54.392278469363433</v>
+      </c>
+      <c r="D41" s="1">
         <f t="shared" si="8"/>
-        <v>5.007444255036746</v>
-      </c>
-      <c r="L32" s="1">
-        <f t="shared" si="8"/>
-        <v>5.003557125691878</v>
-      </c>
-      <c r="M32" s="1">
-        <f t="shared" si="8"/>
-        <v>5.0468770249812334</v>
+        <v>-53.651300936870108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="C42" s="1">
+        <f t="shared" ref="C42:D42" si="9">(C38-C32)/C32*100</f>
+        <v>-56.427864345574307</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="9"/>
+        <v>-59.224089842561433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 3/5/7 order choices, and arbitrary nPointsOnEdge
</commit_message>
<xml_diff>
--- a/doc/Result_Record.xlsx
+++ b/doc/Result_Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Models\FVM\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8DDD44-0E11-47C4-AB1A-3A72CF148F87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5597AA8B-53DE-4B8B-8766-917DDB03831A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5388" yWindow="1110" windowWidth="16650" windowHeight="10206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12636" yWindow="1218" windowWidth="16650" windowHeight="10206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5th" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="10">
   <si>
     <t>L1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1162,6 +1162,145 @@
       <c r="F42" s="1">
         <f t="shared" si="14"/>
         <v>107.82614203259995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>4.5</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0.5</v>
+      </c>
+      <c r="F45">
+        <v>0.25</v>
+      </c>
+      <c r="H45" t="s">
+        <v>6</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>0.5</v>
+      </c>
+      <c r="L45">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1.8451163937782E-5</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2.4984511971875003E-7</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="H46" t="s">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <f>LOG(B46/C46)/LOG(B45/C45)</f>
+        <v>5.305069958862032</v>
+      </c>
+      <c r="J46" s="1" t="e">
+        <f t="shared" ref="J46:J48" si="15">LOG(C46/D46)/LOG(2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" s="1" t="e">
+        <f t="shared" ref="K46:K48" si="16">LOG(D46/E46)/LOG(2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" s="1" t="e">
+        <f t="shared" ref="L46:L48" si="17">LOG(E46/F46)/LOG(2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2.53303185808823E-5</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3.4876270679195201E-7</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="H47" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1">
+        <f>LOG(B47/C47)/LOG(B45/C45)</f>
+        <v>5.2845059497350251</v>
+      </c>
+      <c r="J47" s="1" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" s="1" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="1" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="1">
+        <v>5.0949643402108897E-5</v>
+      </c>
+      <c r="C48" s="1">
+        <v>6.8693521085838898E-7</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="H48" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" s="1">
+        <f>LOG(B48/C48)/LOG(B45/C45)</f>
+        <v>5.3103867300756633</v>
+      </c>
+      <c r="J48" s="1" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K48" s="1" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L48" s="1" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>